<commit_message>
31 Jan 25 update
</commit_message>
<xml_diff>
--- a/data/lab_personnel_timeline.xlsx
+++ b/data/lab_personnel_timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\utku\GitHub\Lab_personnel_timeline\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39074E6B-1049-42E3-9D5A-404950D45BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8EA616-8969-44B2-B2A1-C615E8279077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{894F3479-6172-4C97-B34D-DB9478A5D1D4}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8928" xr2:uid="{894F3479-6172-4C97-B34D-DB9478A5D1D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="181">
   <si>
     <t>Given name</t>
   </si>
@@ -573,6 +573,12 @@
   </si>
   <si>
     <t>Pakbaz</t>
+  </si>
+  <si>
+    <t>Howell</t>
+  </si>
+  <si>
+    <t>Cassie</t>
   </si>
 </sst>
 </file>
@@ -939,21 +945,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2953AC09-9765-4667-A6A5-FD188D0D574B}">
-  <dimension ref="A1:E96"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="E75" sqref="E75"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -970,7 +976,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -987,7 +993,7 @@
         <v>45444</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1004,7 +1010,7 @@
         <v>45292</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1021,7 +1027,7 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1038,7 +1044,7 @@
         <v>45139</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1055,7 +1061,7 @@
         <v>45139</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1072,7 +1078,7 @@
         <v>44682</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1089,7 +1095,7 @@
         <v>44682</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1106,7 +1112,7 @@
         <v>44682</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1123,7 +1129,7 @@
         <v>44317</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1140,7 +1146,7 @@
         <v>44166</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -1157,7 +1163,7 @@
         <v>43739</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1174,7 +1180,7 @@
         <v>43739</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1191,7 +1197,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -1208,7 +1214,7 @@
         <v>43586</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -1225,7 +1231,7 @@
         <v>43586</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1242,7 +1248,7 @@
         <v>43586</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -1259,7 +1265,7 @@
         <v>43344</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1276,7 +1282,7 @@
         <v>43221</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -1293,7 +1299,7 @@
         <v>42856</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -1310,7 +1316,7 @@
         <v>42856</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -1327,7 +1333,7 @@
         <v>42856</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -1344,7 +1350,7 @@
         <v>42856</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -1361,7 +1367,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -1378,7 +1384,7 @@
         <v>42491</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>58</v>
       </c>
@@ -1395,7 +1401,7 @@
         <v>42491</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -1412,7 +1418,7 @@
         <v>42248</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>62</v>
       </c>
@@ -1429,7 +1435,7 @@
         <v>42248</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -1446,7 +1452,7 @@
         <v>42125</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>66</v>
       </c>
@@ -1463,7 +1469,7 @@
         <v>42125</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>68</v>
       </c>
@@ -1480,7 +1486,7 @@
         <v>41974</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>70</v>
       </c>
@@ -1497,7 +1503,7 @@
         <v>41974</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>72</v>
       </c>
@@ -1514,7 +1520,7 @@
         <v>41913</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>74</v>
       </c>
@@ -1531,7 +1537,7 @@
         <v>41913</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>76</v>
       </c>
@@ -1548,7 +1554,7 @@
         <v>41883</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>78</v>
       </c>
@@ -1565,7 +1571,7 @@
         <v>41760</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>80</v>
       </c>
@@ -1582,7 +1588,7 @@
         <v>41760</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>82</v>
       </c>
@@ -1599,7 +1605,7 @@
         <v>41760</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>84</v>
       </c>
@@ -1616,7 +1622,7 @@
         <v>41609</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>86</v>
       </c>
@@ -1633,7 +1639,7 @@
         <v>41395</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>88</v>
       </c>
@@ -1650,7 +1656,7 @@
         <v>41395</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>90</v>
       </c>
@@ -1667,7 +1673,7 @@
         <v>41395</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>74</v>
       </c>
@@ -1684,7 +1690,7 @@
         <v>41395</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>93</v>
       </c>
@@ -1701,7 +1707,7 @@
         <v>41183</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>94</v>
       </c>
@@ -1718,7 +1724,7 @@
         <v>41030</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>96</v>
       </c>
@@ -1735,7 +1741,7 @@
         <v>40817</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>98</v>
       </c>
@@ -1752,7 +1758,7 @@
         <v>40725</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>100</v>
       </c>
@@ -1769,7 +1775,7 @@
         <v>40664</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>102</v>
       </c>
@@ -1786,7 +1792,7 @@
         <v>40664</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>104</v>
       </c>
@@ -1803,7 +1809,7 @@
         <v>40664</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>106</v>
       </c>
@@ -1820,7 +1826,7 @@
         <v>40664</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>108</v>
       </c>
@@ -1837,7 +1843,7 @@
         <v>40513</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>110</v>
       </c>
@@ -1854,7 +1860,7 @@
         <v>40513</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>111</v>
       </c>
@@ -1871,7 +1877,7 @@
         <v>40026</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>113</v>
       </c>
@@ -1888,7 +1894,7 @@
         <v>39934</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>115</v>
       </c>
@@ -1905,7 +1911,7 @@
         <v>39783</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>117</v>
       </c>
@@ -1922,7 +1928,7 @@
         <v>39722</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>82</v>
       </c>
@@ -1939,7 +1945,7 @@
         <v>39722</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>119</v>
       </c>
@@ -1956,7 +1962,7 @@
         <v>39569</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -1973,7 +1979,7 @@
         <v>39569</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>122</v>
       </c>
@@ -1990,7 +1996,7 @@
         <v>39356</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>84</v>
       </c>
@@ -2007,7 +2013,7 @@
         <v>39203</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>5</v>
       </c>
@@ -2024,7 +2030,7 @@
         <v>39052</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>125</v>
       </c>
@@ -2041,7 +2047,7 @@
         <v>38991</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>127</v>
       </c>
@@ -2058,7 +2064,7 @@
         <v>38991</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>45</v>
       </c>
@@ -2075,7 +2081,7 @@
         <v>38991</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>130</v>
       </c>
@@ -2092,7 +2098,7 @@
         <v>38261</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>132</v>
       </c>
@@ -2106,7 +2112,7 @@
         <v>38169</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>134</v>
       </c>
@@ -2123,7 +2129,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>125</v>
       </c>
@@ -2138,7 +2144,7 @@
       </c>
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>138</v>
       </c>
@@ -2153,7 +2159,7 @@
       </c>
       <c r="E71" s="1"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>140</v>
       </c>
@@ -2167,7 +2173,7 @@
         <v>45139</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>142</v>
       </c>
@@ -2181,7 +2187,7 @@
         <v>45444</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>144</v>
       </c>
@@ -2196,7 +2202,7 @@
       </c>
       <c r="E74" s="2"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>146</v>
       </c>
@@ -2213,7 +2219,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>148</v>
       </c>
@@ -2230,7 +2236,7 @@
         <v>45536</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>150</v>
       </c>
@@ -2245,7 +2251,7 @@
       </c>
       <c r="E77" s="2"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>152</v>
       </c>
@@ -2260,7 +2266,7 @@
       </c>
       <c r="E78" s="2"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>154</v>
       </c>
@@ -2275,7 +2281,7 @@
       </c>
       <c r="E79" s="2"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>35</v>
       </c>
@@ -2290,7 +2296,7 @@
       </c>
       <c r="E80" s="2"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>11</v>
       </c>
@@ -2305,7 +2311,7 @@
       </c>
       <c r="E81" s="2"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>11</v>
       </c>
@@ -2320,7 +2326,7 @@
       </c>
       <c r="E82" s="2"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>156</v>
       </c>
@@ -2335,7 +2341,7 @@
       </c>
       <c r="E83" s="2"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>158</v>
       </c>
@@ -2352,7 +2358,7 @@
         <v>45536</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>158</v>
       </c>
@@ -2367,7 +2373,7 @@
       </c>
       <c r="E85" s="2"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>160</v>
       </c>
@@ -2382,7 +2388,7 @@
       </c>
       <c r="E86" s="2"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>162</v>
       </c>
@@ -2397,7 +2403,7 @@
       </c>
       <c r="E87" s="2"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>113</v>
       </c>
@@ -2414,7 +2420,7 @@
         <v>43952</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>113</v>
       </c>
@@ -2428,7 +2434,7 @@
         <v>45292</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>140</v>
       </c>
@@ -2442,7 +2448,7 @@
         <v>45566</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>167</v>
       </c>
@@ -2456,7 +2462,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>169</v>
       </c>
@@ -2470,7 +2476,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>171</v>
       </c>
@@ -2484,7 +2490,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>173</v>
       </c>
@@ -2498,7 +2504,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>175</v>
       </c>
@@ -2512,7 +2518,7 @@
         <v>45597</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>177</v>
       </c>
@@ -2523,6 +2529,20 @@
         <v>27</v>
       </c>
       <c r="D96" s="1">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>180</v>
+      </c>
+      <c r="B97" t="s">
+        <v>179</v>
+      </c>
+      <c r="C97" t="s">
+        <v>16</v>
+      </c>
+      <c r="D97" s="1">
         <v>45658</v>
       </c>
     </row>
@@ -2535,6 +2555,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a">
@@ -2543,15 +2572,6 @@
     <TaxCatchAll xmlns="6cbc0c5a-d948-46e5-8624-1bad210f77c7" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2804,20 +2824,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{052A151B-9EBC-4A5B-80E8-331BB541A51E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDD2033D-62C9-49C5-95D2-9D0E2397323D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
     <ds:schemaRef ds:uri="6cbc0c5a-d948-46e5-8624-1bad210f77c7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{052A151B-9EBC-4A5B-80E8-331BB541A51E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>